<commit_message>
added LEDS, need symbols and footprints to finish work
</commit_message>
<xml_diff>
--- a/diodes.xlsx
+++ b/diodes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Altium-Lib-Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB688A2-7BD7-4991-A740-CDF7B735F00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAB7CAE-F013-4941-ADDB-1A3B7A64355E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9338" xr2:uid="{B0D9C48D-0538-469A-91B8-A1A70C552D06}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9338" activeTab="1" xr2:uid="{B0D9C48D-0538-469A-91B8-A1A70C552D06}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>TPN</t>
   </si>
@@ -156,6 +157,189 @@
   </si>
   <si>
     <t>Library Ref</t>
+  </si>
+  <si>
+    <t>LED RED DIFFUSED T-1 3/4 T/H</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Lens Color</t>
+  </si>
+  <si>
+    <t>Lens Transparency</t>
+  </si>
+  <si>
+    <t>Diffused</t>
+  </si>
+  <si>
+    <t>Millicandela Rating</t>
+  </si>
+  <si>
+    <t>19mcd</t>
+  </si>
+  <si>
+    <t>Lens Style</t>
+  </si>
+  <si>
+    <t>Round with Domed Top</t>
+  </si>
+  <si>
+    <t>Lens Size</t>
+  </si>
+  <si>
+    <t>5mm, T-1 3/4</t>
+  </si>
+  <si>
+    <t>Voltage - Forward (Vf) (Typ)</t>
+  </si>
+  <si>
+    <t>2V</t>
+  </si>
+  <si>
+    <t>Current - Test</t>
+  </si>
+  <si>
+    <t>10mA</t>
+  </si>
+  <si>
+    <t>Viewing Angle</t>
+  </si>
+  <si>
+    <t>36°</t>
+  </si>
+  <si>
+    <t>LED-Red</t>
+  </si>
+  <si>
+    <t>Wavelength - Dominant</t>
+  </si>
+  <si>
+    <t>Wavelength - Peak</t>
+  </si>
+  <si>
+    <t>Supplier Device Package</t>
+  </si>
+  <si>
+    <t>Size / Dimension</t>
+  </si>
+  <si>
+    <t>Height (Max)</t>
+  </si>
+  <si>
+    <t>623nm</t>
+  </si>
+  <si>
+    <t>635nm</t>
+  </si>
+  <si>
+    <t>Radial</t>
+  </si>
+  <si>
+    <t>T-1 3/4</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>8.60mm</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>LTL-4223</t>
+  </si>
+  <si>
+    <t>160-1127-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTL-4223/160-1127-ND/200395</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR 5MM ROUND T/H</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Colorless</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>7065mcd</t>
+  </si>
+  <si>
+    <t>5.0mm Dia</t>
+  </si>
+  <si>
+    <t>3.2V</t>
+  </si>
+  <si>
+    <t>20mA</t>
+  </si>
+  <si>
+    <t>30°</t>
+  </si>
+  <si>
+    <t>5-mm Round</t>
+  </si>
+  <si>
+    <t>LED-Blue</t>
+  </si>
+  <si>
+    <t>Cree Inc.</t>
+  </si>
+  <si>
+    <t>C503B-BCN-CV0Z0461</t>
+  </si>
+  <si>
+    <t>C503B-BCN-CV0Z0461-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/cree-inc/C503B-BCN-CV0Z0461/C503B-BCN-CV0Z0461-ND/1922945</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR T-1 3/4 T/H</t>
+  </si>
+  <si>
+    <t>1200mcd</t>
+  </si>
+  <si>
+    <t>3.5V</t>
+  </si>
+  <si>
+    <t>470nm</t>
+  </si>
+  <si>
+    <t>468nm</t>
+  </si>
+  <si>
+    <t>8.70mm</t>
+  </si>
+  <si>
+    <t>LTL2T3TBK5</t>
+  </si>
+  <si>
+    <t>160-1610-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTL2T3TBK5/160-1610-ND/573515</t>
   </si>
 </sst>
 </file>
@@ -519,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B2D707-FBE2-4146-806D-2EE3BFD44B41}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -665,4 +849,358 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F7FB38-E69D-481E-80F3-8BBB83E647A4}">
+  <dimension ref="A1:AE4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A2" t="str">
+        <f>"LED-"&amp;TEXT(ROW()-1,"000000")</f>
+        <v>LED-000001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A4" si="0">"LED-"&amp;TEXT(ROW()-1,"000000")</f>
+        <v>LED-000002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>LED-000003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>70</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" t="s">
+        <v>99</v>
+      </c>
+      <c r="U4" t="s">
+        <v>89</v>
+      </c>
+      <c r="W4" t="s">
+        <v>75</v>
+      </c>
+      <c r="X4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated diodes library with basic 5mm LEDs, generic symbols, and 1N914
</commit_message>
<xml_diff>
--- a/diodes.xlsx
+++ b/diodes.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Altium-Lib-Tom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrne\Altium-Lib-Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAB7CAE-F013-4941-ADDB-1A3B7A64355E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51428524-7E37-44D5-8058-477B35053EA1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9338" activeTab="1" xr2:uid="{B0D9C48D-0538-469A-91B8-A1A70C552D06}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="9345" xr2:uid="{B0D9C48D-0538-469A-91B8-A1A70C552D06}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="LED" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="102">
   <si>
     <t>TPN</t>
   </si>
@@ -150,12 +150,6 @@
     <t>Operating Temperature - Junction</t>
   </si>
   <si>
-    <t>DIO</t>
-  </si>
-  <si>
-    <t>DIO-TH</t>
-  </si>
-  <si>
     <t>Library Ref</t>
   </si>
   <si>
@@ -340,6 +334,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTL2T3TBK5/160-1610-ND/573515</t>
+  </si>
+  <si>
+    <t>DIO-GEN</t>
   </si>
 </sst>
 </file>
@@ -703,16 +700,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B2D707-FBE2-4146-806D-2EE3BFD44B41}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +752,7 @@
         <v>38</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -786,7 +785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>"DIO-"&amp;TEXT(ROW()-1,"000000")</f>
         <v>DIO-000001</v>
@@ -825,10 +824,10 @@
         <v>37</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="O2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="P2" t="s">
         <v>11</v>
@@ -855,13 +854,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F7FB38-E69D-481E-80F3-8BBB83E647A4}">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,61 +882,61 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>2</v>
@@ -956,247 +969,247 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>"LED-"&amp;TEXT(ROW()-1,"000000")</f>
         <v>LED-000001</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>55</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>59</v>
-      </c>
-      <c r="L2" t="s">
-        <v>61</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
       </c>
       <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" t="s">
         <v>68</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>69</v>
       </c>
-      <c r="P2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>70</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>71</v>
       </c>
-      <c r="S2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" t="s">
         <v>73</v>
       </c>
-      <c r="U2" t="s">
-        <v>62</v>
-      </c>
-      <c r="W2" t="s">
-        <v>75</v>
-      </c>
       <c r="X2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Y2" t="s">
         <v>13</v>
       </c>
       <c r="Z2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A4" si="0">"LED-"&amp;TEXT(ROW()-1,"000000")</f>
         <v>LED-000002</v>
       </c>
       <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
         <v>82</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>83</v>
       </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>84</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>85</v>
-      </c>
-      <c r="K3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" t="s">
-        <v>87</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" t="s">
         <v>70</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W3" t="s">
         <v>88</v>
       </c>
-      <c r="S3" t="s">
-        <v>72</v>
-      </c>
-      <c r="T3" t="s">
-        <v>73</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>89</v>
-      </c>
-      <c r="W3" t="s">
-        <v>90</v>
-      </c>
-      <c r="X3" t="s">
-        <v>91</v>
       </c>
       <c r="Y3" t="s">
         <v>13</v>
       </c>
       <c r="Z3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>LED-000003</v>
       </c>
       <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" t="s">
-        <v>96</v>
-      </c>
       <c r="K4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M4" t="s">
         <v>34</v>
       </c>
       <c r="N4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" t="s">
+        <v>96</v>
+      </c>
+      <c r="P4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" t="s">
         <v>97</v>
       </c>
-      <c r="O4" t="s">
+      <c r="U4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" t="s">
+        <v>73</v>
+      </c>
+      <c r="X4" t="s">
         <v>98</v>
-      </c>
-      <c r="P4" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>70</v>
-      </c>
-      <c r="R4" t="s">
-        <v>71</v>
-      </c>
-      <c r="S4" t="s">
-        <v>72</v>
-      </c>
-      <c r="T4" t="s">
-        <v>99</v>
-      </c>
-      <c r="U4" t="s">
-        <v>89</v>
-      </c>
-      <c r="W4" t="s">
-        <v>75</v>
-      </c>
-      <c r="X4" t="s">
-        <v>100</v>
       </c>
       <c r="Y4" t="s">
         <v>13</v>
       </c>
       <c r="Z4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AA4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>